<commit_message>
Klar för dagen 12/6
</commit_message>
<xml_diff>
--- a/Kravlista.xlsx
+++ b/Kravlista.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Krav</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Anton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kund </t>
+  </si>
+  <si>
+    <t>AF 2.1 Administrera medlemmar</t>
+  </si>
+  <si>
+    <t>Gymansvarig</t>
+  </si>
+  <si>
+    <t>BK 2 ,BK 2.2</t>
   </si>
 </sst>
 </file>
@@ -386,15 +398,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F5"/>
+  <dimension ref="A2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -422,6 +436,9 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
@@ -433,8 +450,14 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" t="s">
         <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -444,11 +467,31 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
       <c r="F5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>